<commit_message>
Implementando LOG e Asserto de formulário de login
</commit_message>
<xml_diff>
--- a/media/xlsx/corretiva.xlsx
+++ b/media/xlsx/corretiva.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CIES-10956</t>
+          <t>CIES-11816</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -483,17 +483,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Todas as câmeras do site estão offline</t>
+          <t>todas as câmeras do p0110 estão off-line</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Max Costa Machado</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>P0092-PCL PK-BAI</t>
+          <t>P0110-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -510,27 +510,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CIES-10958</t>
+          <t>CIES-11817</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0120</t>
+          <t>câmeras do p0035 estão off-line</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>P0120-PCL-PK-SER</t>
+          <t>P0035-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -547,27 +547,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CIES-10959</t>
+          <t>CIES-11830</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0122</t>
+          <t>Ajuste de posicionamento de câmera</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>Max Costa Machado</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>P0122-PCL-PK-SER</t>
+          <t>P0036-PCL-PK-VVE</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -584,32 +584,32 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CIES-11244</t>
+          <t>CIES-11833</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0071</t>
+          <t>câmeras do p0134  estão  off-line</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>P0071-PCL-PK-CAR</t>
+          <t>P0134-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>NO PRAZO</t>
+          <t>FORA DO PRAZO</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -621,27 +621,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CIES-11245</t>
+          <t>CIES-11836</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 2</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0118</t>
+          <t>Ajuste de posicionamento de câmera</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>Max Costa Machado</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>P0118-PCL-PK-SER</t>
+          <t>P0132-PK-VLS-SER</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -658,27 +658,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CIES-11246</t>
+          <t>CIES-11837</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 3</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0119</t>
+          <t xml:space="preserve">câmeras do p0062 está com galhos a frente. </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>P0119-PCL-PK-SER</t>
+          <t>P0062-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -695,7 +695,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CIES-11247</t>
+          <t>CIES-11838</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -705,17 +705,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0119</t>
+          <t>A câmera foi colocada atrás de uma placa, dificultando a visualização dos veículos.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>P0119-PCL-PK-SER</t>
+          <t>P0112-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -732,7 +732,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CIES-11248</t>
+          <t>CIES-12142</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -742,7 +742,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0120</t>
+          <t>CORRETIVA SITE P0033</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -752,7 +752,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>P0120-PCL-PK-SER</t>
+          <t>P0033-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -769,7 +769,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CIES-11249</t>
+          <t>CIES-12143</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0122</t>
+          <t>CORRETIVA SITE P0115</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -789,7 +789,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>P0122-PCL-PK-SER</t>
+          <t>P0115-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -806,7 +806,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CIES-11261</t>
+          <t>CIES-12144</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -816,7 +816,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0088</t>
+          <t>CORRETIVA SITE P0120</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -826,7 +826,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>P0086-PCL-PK-VIA</t>
+          <t>P0120-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -843,7 +843,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CIES-11262</t>
+          <t>CIES-12145</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0088</t>
+          <t>CORRETIVA SITE P0122</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -863,7 +863,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>P0088-PCL-PK-VIA</t>
+          <t>P0122-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -880,7 +880,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CIES-11263</t>
+          <t>CIES-12150</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -890,7 +890,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0089</t>
+          <t>P0124 - Site sem acesso</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -900,7 +900,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>P0089-PCL-PK-VIA</t>
+          <t>P0124-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -917,7 +917,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CIES-11264</t>
+          <t>CIES-12154</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -927,7 +927,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>P0030 - Todas as câmeras offline</t>
+          <t>CORRETIVA SITE P0078</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -937,7 +937,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>P0030-PCL-PK-CAR</t>
+          <t>P0078-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -954,7 +954,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CIES-11265</t>
+          <t>CIES-12156</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -964,7 +964,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">P0122 - SITE SEM ACESSO EXTERNO </t>
+          <t>CORRETIVA SITE P0028</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -974,7 +974,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>P0122-PCL-PK-SER</t>
+          <t>P0028-PCL-PK-VVE</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -991,7 +991,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CIES-11266</t>
+          <t>CIES-12159</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1001,17 +1001,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>P0148 - Corretiva Site Off</t>
+          <t>todas as câmeras do p0038 estão off-line</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>P0148-PCL-PK-FUN</t>
+          <t>P0038-PCL-PK-VVE</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CIES-11267</t>
+          <t>CIES-12161</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">P0126 - SITE SEM ACESSO EXTERNO </t>
+          <t>CORRETIVA SITE P0122</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>P0126-PCL-PK-SER</t>
+          <t>P0122-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1065,7 +1065,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CIES-11268</t>
+          <t>CIES-12164</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>P0129 - CORRETIVA SITE SEM ACESSO EXTERNO</t>
+          <t>CORRETIVA SITE P0002</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1085,7 +1085,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>P0129-PCL-PK-SER</t>
+          <t>P0002-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1102,7 +1102,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CIES-11269</t>
+          <t>CIES-12165</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>SITE FORA DO AR - P0116</t>
+          <t>CORRETIVA SITE P0129</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1122,7 +1122,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>P0116-PCL-PK-SER</t>
+          <t>P0129-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1139,7 +1139,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CIES-11270</t>
+          <t>CIES-12166</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>TODAS AS CÂMERAS ESTÃO OFFLINE - P0143</t>
+          <t>CORRETIVA SITE P0290</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>P0143-PCL-PK-SER</t>
+          <t>P0290-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1176,7 +1176,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CIES-11271</t>
+          <t>CIES-12167</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0120</t>
+          <t>CORRETIVA SITE P0006</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>P0120-PCL-PK-SER</t>
+          <t>P0006-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1213,7 +1213,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CIES-11272</t>
+          <t>CIES-12169</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0078</t>
+          <t>CORRETIVA SITE P0033</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>P0078-PCL-PK-CAR</t>
+          <t>P0033-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1250,7 +1250,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CIES-11273</t>
+          <t>CIES-12170</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0118</t>
+          <t>CORRETIVA SITE P0091</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>P0118-PCL-PK-SER</t>
+          <t>P0091-PCL-PK-VIA</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1287,7 +1287,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CIES-11275</t>
+          <t>CIES-12175</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1297,17 +1297,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0119</t>
+          <t xml:space="preserve">todas as câmeras do p0052 estão off-line   </t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>P0119-PCL-PK-SER</t>
+          <t>P0052-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1324,7 +1324,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CIES-11276</t>
+          <t>CIES-12176</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1334,17 +1334,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0146</t>
+          <t xml:space="preserve">todas as câmeras do p0001 estão off-line   </t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>P0146-PCL-PK-SER</t>
+          <t>P0001-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1361,7 +1361,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CIES-11281</t>
+          <t>CIES-12177</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0123 estão off-line </t>
+          <t xml:space="preserve">todas as câmeras do p0122 estão off-line   </t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>P0123-PCL-PK-SER</t>
+          <t>P0122-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1398,7 +1398,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CIES-11282</t>
+          <t>CIES-12178</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0120 estão off-line </t>
+          <t xml:space="preserve">todas as câmeras do p0050 estão off-line   </t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>P0120-PCL-PK-SER</t>
+          <t>P0050-PCL-PK-VVE</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1435,7 +1435,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CIES-11297</t>
+          <t>CIES-12182</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0120</t>
+          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0006</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1455,7 +1455,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>P0120-PCL-PK-SER</t>
+          <t>P0006-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1472,17 +1472,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CIES-11298</t>
+          <t>CIES-12215</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 2</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0119</t>
+          <t>CORRETIVA SITE P0005</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>P0119-PCL-PK-SER</t>
+          <t>P0005-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1509,17 +1509,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CIES-11299</t>
+          <t>CIES-12216</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 2</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0122</t>
+          <t>CORRETIVA SITE P0010</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>P0122-PCL-PK-SER</t>
+          <t>P0010-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1546,7 +1546,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CIES-11318</t>
+          <t>CIES-12217</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO  - P0122</t>
+          <t>CORRETIVA SITE P0122</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1583,7 +1583,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CIES-11319</t>
+          <t>CIES-12230</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1593,7 +1593,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0119</t>
+          <t>CORRETIVA SITE P0122</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>P0119-PCL-PK-SER</t>
+          <t>P0122-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1612,746 +1612,6 @@
         </is>
       </c>
       <c r="G32" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>CIES-11321</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0109</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>P0109-PCL-PK-SER</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>CIES-11322</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0129</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>P0129-PCL-PK-SER</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>CIES-11324</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0148</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>P0148-PCL-PK-FUN</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>CIES-11327</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t xml:space="preserve">todas as câmeras do p0138 estão off-line  </t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>P0138-PCL-PK-SER</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>CIES-11329</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>CORRETIVA - SITE SEM ACESSO - P0094</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>P0094-PCL-PK-VIA</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>CIES-11331</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Prioridade 3</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Corretiva - Câmera de contexto offline</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>P0165-PK-VLS-BAR</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>CIES-11340</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Prioridade 2</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>CORRETIVA - CAMERA SEM ACESSO EXTERNO - LPR2 - P0055</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>P0055-PCL-PK-CAR</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>CIES-11341</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0126</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>P0126-PCL-PK-SER</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>CIES-11342</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0133</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>P0133-PCL-PK-SER</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>CIES-11343</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>P0121 - SITE OFFLINE</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>P0121-PCL-PK-SER</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>CIES-11344</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">todas as câmeras do p0023 estão off-line    </t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>P0023-PCL-PK-GRP</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>FORA DO PRAZO</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>CIES-11345</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t xml:space="preserve">todas as câmeras do p0133 estão off-line    </t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>P0133-PCL-PK-SER</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>CIES-11346</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t xml:space="preserve">todas as câmeras do p0134 estão off-line    </t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>P0134-PCL-PK-SER</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>CIES-11351</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Prioridade 2</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>SER-P0129-LPR2-SAI-RUA-ABREUAMORIMMACHADO</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Max Costa Machado</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>P0129-PCL-PK-SER</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>CIES-11369</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Prioridade 2</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>CORRETIVA - CÂMERAS DE ENTRADA OFFLINE</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>P0032-PCL-PK-VVE</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>CIES-11370</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Prioridade 2</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>CORRETIVA - UMA CÂMERA LPR OFFLINE</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>P0064-PCL-PK-CAR</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>CIES-11372</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>CORRETIVA - TODO O SITE OFFLINE</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>P0021-PCL-PK-GRP</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>CIES-11384</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>P0290 - SITE OFFLINE</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>P0290-PCL-PK-SER</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>CIES-11385</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>P0119 - Site Fora</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>P0119-PCL-PK-SER</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>CIES-11386</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Prioridade 1</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>P0252 - Site Fora</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Service Desk Perkons</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>P0252-PCL-PK-VVE</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
         <is>
           <t>NO PRAZO</t>
         </is>

</xml_diff>

<commit_message>
Realizando alteraçõe estruturais no projeto
</commit_message>
<xml_diff>
--- a/media/xlsx/corretiva.xlsx
+++ b/media/xlsx/corretiva.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CIES-11816</t>
+          <t>CIES-12568</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -483,17 +483,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>todas as câmeras do p0110 estão off-line</t>
+          <t>CORRETIVA SITE P0131</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>P0110-PCL-PK-SER</t>
+          <t>P0131-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -510,7 +510,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CIES-11817</t>
+          <t>CIES-12569</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -520,17 +520,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>câmeras do p0035 estão off-line</t>
+          <t>CORRETIVA SITE P0078</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>P0035-PCL-PK-CAR</t>
+          <t>P0078-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -547,27 +547,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CIES-11830</t>
+          <t>CIES-12570</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Prioridade 2</t>
+          <t>Prioridade 1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ajuste de posicionamento de câmera</t>
+          <t>CORRETIVA SITE P0129</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Max Costa Machado</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>P0036-PCL-PK-VVE</t>
+          <t>P0129-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -584,7 +584,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CIES-11833</t>
+          <t>CIES-12585</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -594,7 +594,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>câmeras do p0134  estão  off-line</t>
+          <t>CÂMERAS DO P0071 ESTÃO OFF-LINE</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -604,12 +604,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>P0134-PCL-PK-SER</t>
+          <t>P0071-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>FORA DO PRAZO</t>
+          <t>NO PRAZO</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -621,27 +621,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CIES-11836</t>
+          <t>CIES-12586</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Prioridade 2</t>
+          <t>Prioridade 1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ajuste de posicionamento de câmera</t>
+          <t xml:space="preserve">todas as câmeras do p0073 estão off-line  </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Max Costa Machado</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>P0132-PK-VLS-SER</t>
+          <t>P0073-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -658,17 +658,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CIES-11837</t>
+          <t>CIES-12587</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Prioridade 3</t>
+          <t>Prioridade 1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">câmeras do p0062 está com galhos a frente. </t>
+          <t xml:space="preserve">todas as câmeras do p0077 estão off-line  </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>P0062-PCL-PK-CAR</t>
+          <t>P0077-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -695,7 +695,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CIES-11838</t>
+          <t>CIES-12588</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -705,7 +705,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>A câmera foi colocada atrás de uma placa, dificultando a visualização dos veículos.</t>
+          <t xml:space="preserve">todas as câmeras do p0122 estão off-line  </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -715,7 +715,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>P0112-PCL-PK-SER</t>
+          <t>P0122-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -732,7 +732,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CIES-12142</t>
+          <t>CIES-12589</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -742,17 +742,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0033</t>
+          <t xml:space="preserve">todas as câmeras do p0128 estão off-line  </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>P0033-PCL-PK-CAR</t>
+          <t>P0128-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -762,14 +762,14 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>NO PRAZO</t>
+          <t>FORA DO PRAZO</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CIES-12143</t>
+          <t>CIES-12600</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -779,17 +779,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0115</t>
+          <t>todas as câmeras do p077 estão off-line</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>P0115-PCL-PK-SER</t>
+          <t>P0077-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -806,7 +806,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CIES-12144</t>
+          <t>CIES-12601</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -816,17 +816,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0120</t>
+          <t>todas as câmeras do p0148  estão off-line</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>P0120-PCL-PK-SER</t>
+          <t>P0148-PCL-PK-FUN</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -843,7 +843,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CIES-12145</t>
+          <t>CIES-12602</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -853,17 +853,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0122</t>
+          <t>todas as câmeras do p0017 estão off-line</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>P0122-PCL-PK-SER</t>
+          <t>P0017-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -880,7 +880,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CIES-12150</t>
+          <t>CIES-12603</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -890,17 +890,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>P0124 - Site sem acesso</t>
+          <t>todas as câmeras do p0091 estão off-line</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>P0124-PCL-PK-SER</t>
+          <t>P0091-PCL-PK-VIA</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -917,7 +917,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CIES-12154</t>
+          <t>CIES-12608</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -927,7 +927,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0078</t>
+          <t>CORRETIVA SITE P0129</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -937,7 +937,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>P0078-PCL-PK-CAR</t>
+          <t>P0129-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -954,7 +954,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CIES-12156</t>
+          <t>CIES-12614</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -964,7 +964,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0028</t>
+          <t>CORRETIVA SITE P0001</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -974,7 +974,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>P0028-PCL-PK-VVE</t>
+          <t>P0001-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -991,7 +991,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CIES-12159</t>
+          <t>CIES-12615</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1001,17 +1001,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>todas as câmeras do p0038 estão off-line</t>
+          <t>CORRETIVA SITE P0014</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>P0038-PCL-PK-VVE</t>
+          <t>P0014-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CIES-12161</t>
+          <t>CIES-12618</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1065,17 +1065,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CIES-12164</t>
+          <t>CIES-12619</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 3</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0002</t>
+          <t>CORRETIVA SITE P0014</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1085,7 +1085,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>P0002-PCL-PK-GRP</t>
+          <t>P0014-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1102,7 +1102,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CIES-12165</t>
+          <t>CIES-12620</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0129</t>
+          <t>CORRETIVA SITE P0120</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1122,7 +1122,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>P0129-PCL-PK-SER</t>
+          <t>P0120-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1139,7 +1139,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CIES-12166</t>
+          <t>CIES-12622</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0290</t>
+          <t>CORRETIVA SITE P0122</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>P0290-PCL-PK-SER</t>
+          <t>P0122-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1176,7 +1176,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CIES-12167</t>
+          <t>CIES-12624</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0006</t>
+          <t>CORRETIVA SITE P0012</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>P0006-PCL-PK-GRP</t>
+          <t>P0012-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1213,7 +1213,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CIES-12169</t>
+          <t>CIES-12625</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0033</t>
+          <t>CORRETIVA SITE P0112</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>P0033-PCL-PK-CAR</t>
+          <t>P0112-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1250,7 +1250,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CIES-12170</t>
+          <t>CIES-12626</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0091</t>
+          <t>CORRETIVA SITE P0021</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>P0091-PCL-PK-VIA</t>
+          <t>P0021-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1287,7 +1287,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CIES-12175</t>
+          <t>CIES-12629</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1297,17 +1297,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0052 estão off-line   </t>
+          <t>CORRETIVA SITE P0150</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>P0052-PCL-PK-CAR</t>
+          <t>P0150-PCL-PK-FUN</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1324,7 +1324,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CIES-12176</t>
+          <t>CIES-12630</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1334,17 +1334,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0001 estão off-line   </t>
+          <t>CORRETIVA SITE P0129</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>P0001-PCL-PK-GRP</t>
+          <t>P0129-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1361,7 +1361,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CIES-12177</t>
+          <t>CIES-12631</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1371,17 +1371,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0122 estão off-line   </t>
+          <t>CORRETIVA SITE P0150</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>P0122-PCL-PK-SER</t>
+          <t>P0150-PCL-PK-FUN</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1398,7 +1398,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CIES-12178</t>
+          <t>CIES-12632</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1408,17 +1408,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0050 estão off-line   </t>
+          <t>CORRETIVA SITE P0122</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>P0050-PCL-PK-VVE</t>
+          <t>P0122-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1435,7 +1435,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CIES-12182</t>
+          <t>CIES-12633</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CORRETIVA - SITE SEM ACESSO EXTERNO - P0006</t>
+          <t>CORRETIVA SITE P0129</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1455,7 +1455,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>P0006-PCL-PK-GRP</t>
+          <t>P0129-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1472,17 +1472,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CIES-12215</t>
+          <t>CIES-12634</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Prioridade 2</t>
+          <t>Prioridade 1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0005</t>
+          <t>CORRETIVA SITE P0120</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>P0005-PCL-PK-GRP</t>
+          <t>P0120-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1509,17 +1509,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CIES-12216</t>
+          <t>CIES-12636</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Prioridade 2</t>
+          <t>Prioridade 1</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0010</t>
+          <t>CORRETIVA SITE P0033</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>P0010-PCL-PK-GRP</t>
+          <t>P0033-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1546,7 +1546,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CIES-12217</t>
+          <t>CIES-12637</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0122</t>
+          <t>CORRETIVA SITE P0290</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>P0122-PCL-PK-SER</t>
+          <t>P0290-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1583,7 +1583,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CIES-12230</t>
+          <t>CIES-12638</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1593,7 +1593,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0122</t>
+          <t xml:space="preserve">CORRETIVA SITE P0076 </t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1603,15 +1603,866 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
+          <t>P0076-PCL-PK-CAR</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CIES-12639</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">todas as câmeras do p0148 estão off-line </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>P0148-PCL-PK-FUN</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>FORA DO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CIES-12640</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">todas as câmeras do p0147 estão off-line </t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>P0147-PCL-PK-FUN</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CIES-12641</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">todas as câmeras do p0095 estão off-line </t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>P0095-PCL-PK-AFO</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>CIES-12644</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>CORRETIVA SITE P0177</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>P0177-PK-VLS-SER</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>CIES-12645</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>CORRETIVA SITE P0141</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>P0141-PK-VLS-SER</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CIES-12646</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>CORRETIVA SITE P0133</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>P0133-PCL-PK-SER</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>CIES-12648</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0150</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>P0150-PCL-PK-FUN</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CIES-12649</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0129</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>P0129-PCL-PK-SER</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CIES-12650</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0290</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>P0290-PCL-PK-SER</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>CIES-12652</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0087</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>P0087-PCL-PK-VIA</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>CIES-12653</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0090</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>P0090-PCL-PK-VIA</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>CIES-12654</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>CORRETIVA SITE P0060</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>P0060-PCL-PK-CAR</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>CIES-12672</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0170</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>P0170-PK-VLS-MIM</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CIES-12673</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0130</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>P0130-PCL-PK-SER</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CIES-12702</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0198</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>P0198-PK-VLS-GRP</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CIES-12712</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">todas as câmeras do p0068 estão off-line   </t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>P0068-PCL-PK-CAR</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CIES-12713</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">todas as câmeras do p0068 estão off-line   </t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>P0069-PCL-PK-CAR</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>CIES-12714</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">todas as câmeras do p0208 estão off-line   </t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>P0208-PK-VLS-SER</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CIES-12729</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0150</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>P0150-PCL-PK-FUN</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>CIES-12730</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0120</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>P0120-PCL-PK-SER</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>CIES-12731</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0122</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
           <t>P0122-PCL-PK-SER</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>NO PRAZO</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>CIES-12732</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0129</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>P0129-PCL-PK-SER</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>CIES-12733</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0160</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>P0160-PCL-PK-FUN</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
         <is>
           <t>NO PRAZO</t>
         </is>

</xml_diff>

<commit_message>
New Feature: CRUD acompanhamento de ocorrências com processadores
</commit_message>
<xml_diff>
--- a/media/xlsx/corretiva.xlsx
+++ b/media/xlsx/corretiva.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CIES-12568</t>
+          <t>CIES-15731</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0131</t>
+          <t>todas as câmeras do P0146 estão offline</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -493,7 +493,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>P0131-PCL-PK-SER</t>
+          <t>P0146-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -503,24 +503,24 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>NO PRAZO</t>
+          <t>FORA DO PRAZO</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CIES-12569</t>
+          <t>CIES-15733</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Prioridade 2</t>
+          <t>Prioridade 1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0078</t>
+          <t>P0150 - corretiva - site sem acesso</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -530,7 +530,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>P0078-PCL-PK-CAR</t>
+          <t>P0150-PCL-PK-FUN</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -547,7 +547,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CIES-12570</t>
+          <t>CIES-15734</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -557,7 +557,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0129</t>
+          <t>P0091 - Corretiva - Site sem acesso externo</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>P0129-PCL-PK-SER</t>
+          <t>P0091-PCL-PK-VIA</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -584,27 +584,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CIES-12585</t>
+          <t>CIES-15736</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Prioridade 2</t>
+          <t>Prioridade 1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CÂMERAS DO P0071 ESTÃO OFF-LINE</t>
+          <t xml:space="preserve">P0092 - SITE SEM ACESSO EXTERNO </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>P0071-PCL-PK-CAR</t>
+          <t>P0092-PCL-PK-BAI</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -621,7 +621,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CIES-12586</t>
+          <t>CIES-15743</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0073 estão off-line  </t>
+          <t xml:space="preserve">todas as câmeras do p0171 estão off-line  </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>P0073-PCL-PK-CAR</t>
+          <t>P0171-PK-VLS-PRE</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -651,24 +651,24 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>NO PRAZO</t>
+          <t>FORA DO PRAZO</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CIES-12587</t>
+          <t>CIES-15749</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 2</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0077 estão off-line  </t>
+          <t>câmeras do p0 117 estão off-line</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>P0077-PCL-PK-CAR</t>
+          <t>P0117-PCL-PK-ECO</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -688,14 +688,14 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>NO PRAZO</t>
+          <t>FORA DO PRAZO</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CIES-12588</t>
+          <t>CIES-15750</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -705,7 +705,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0122 estão off-line  </t>
+          <t xml:space="preserve">todas as câmeras do p0021  estão off-line  </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -715,7 +715,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>P0122-PCL-PK-SER</t>
+          <t>P0021-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -725,14 +725,14 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>NO PRAZO</t>
+          <t>FORA DO PRAZO</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CIES-12589</t>
+          <t>CIES-15751</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -742,7 +742,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0128 estão off-line  </t>
+          <t xml:space="preserve">todas as câmeras do p0119  estão off-line  </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -752,7 +752,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>P0128-PCL-PK-SER</t>
+          <t>P0119-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -769,7 +769,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CIES-12600</t>
+          <t>CIES-15753</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>todas as câmeras do p077 estão off-line</t>
+          <t xml:space="preserve">todas as câmeras do p0209  estão off-line  </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -789,7 +789,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>P0077-PCL-PK-CAR</t>
+          <t>P0209-PK-VLS-VVE</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -806,7 +806,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CIES-12601</t>
+          <t>CIES-15754</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -816,7 +816,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>todas as câmeras do p0148  estão off-line</t>
+          <t xml:space="preserve">todas as câmeras do p0252 estão off-line  </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -826,7 +826,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>P0148-PCL-PK-FUN</t>
+          <t>P0252-PCL-PK-VVE</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -843,7 +843,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CIES-12602</t>
+          <t>CIES-15755</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -853,17 +853,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>todas as câmeras do p0017 estão off-line</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0147</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>P0017-PCL-PK-GRP</t>
+          <t>P0147-PCL-PK-FUN</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -880,7 +880,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CIES-12603</t>
+          <t>CIES-15756</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -890,17 +890,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>todas as câmeras do p0091 estão off-line</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0150</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>P0091-PCL-PK-VIA</t>
+          <t>P0150-PCL-PK-FUN</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -917,7 +917,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CIES-12608</t>
+          <t>CIES-15757</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -927,7 +927,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0129</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0122</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -937,7 +937,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>P0129-PCL-PK-SER</t>
+          <t>P0122-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -954,7 +954,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CIES-12614</t>
+          <t>CIES-15758</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -964,7 +964,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0001</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0034</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -974,7 +974,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>P0001-PCL-PK-GRP</t>
+          <t>P0034-PCL-PK-VVE</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -991,7 +991,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CIES-12615</t>
+          <t>CIES-15763</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0014</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0091</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>P0014-PCL-PK-GRP</t>
+          <t>P0091-PCL-PK-VIA</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1028,27 +1028,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CIES-12618</t>
+          <t>CIES-16692</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 3</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0122</t>
+          <t xml:space="preserve">CÂMERA DO P0 164 LPR 1 TODA  BRANCA </t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>P0122-PCL-PK-SER</t>
+          <t>P0164-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1065,17 +1065,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CIES-12619</t>
+          <t>CIES-16694</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Prioridade 3</t>
+          <t>Prioridade 1</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0014</t>
+          <t>P0120 - Corretiva - Site sem acesso externo</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1085,7 +1085,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>P0014-PCL-PK-GRP</t>
+          <t>P0120-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1102,7 +1102,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CIES-12620</t>
+          <t>CIES-16695</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0120</t>
+          <t>P0091 - Corretiva - Site sem Acesso Remoto</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1122,7 +1122,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>P0120-PCL-PK-SER</t>
+          <t>P0091-PCL-PK-VIA</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1139,7 +1139,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CIES-12622</t>
+          <t>CIES-16696</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0122</t>
+          <t xml:space="preserve">P0092 - Corretiva - Site sem acesso externo. </t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>P0122-PCL-PK-SER</t>
+          <t>P0092-PCL-PK-BAI</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1176,7 +1176,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CIES-12624</t>
+          <t>CIES-16699</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0012</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0115</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>P0012-PCL-PK-GRP</t>
+          <t>P0115-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1213,7 +1213,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CIES-12625</t>
+          <t>CIES-16700</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0112</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0091</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>P0112-PCL-PK-SER</t>
+          <t>P0091-PCL-PK-VIA</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1250,27 +1250,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CIES-12626</t>
+          <t>CIES-16708</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 3</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0021</t>
+          <t>câmera do p010 está com galhos a frente</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>P0021-PCL-PK-GRP</t>
+          <t>P0010-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1287,7 +1287,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CIES-12629</t>
+          <t>CIES-16709</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0150</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0091</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1307,7 +1307,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>P0150-PCL-PK-FUN</t>
+          <t>P0091-PCL-PK-VIA</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1324,7 +1324,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CIES-12630</t>
+          <t>CIES-16710</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0129</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0092</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>P0129-PCL-PK-SER</t>
+          <t>P0092-PCL-PK-BAI</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1361,27 +1361,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CIES-12631</t>
+          <t>CIES-16713</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 3</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0150</t>
+          <t>câmera do p0015 com galhos a frente</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>P0150-PCL-PK-FUN</t>
+          <t>P0015-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1398,27 +1398,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CIES-12632</t>
+          <t>CIES-16714</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 3</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0122</t>
+          <t>câmera do p0136 com galhos a frente</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>P0122-PCL-PK-SER</t>
+          <t>P0136-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1435,27 +1435,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CIES-12633</t>
+          <t>CIES-16715</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 3</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0129</t>
+          <t>câmera do p0145 com galhos a frente</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>P0129-PCL-PK-SER</t>
+          <t>P0145-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1472,7 +1472,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CIES-12634</t>
+          <t>CIES-16718</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1482,7 +1482,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0120</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0122</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>P0120-PCL-PK-SER</t>
+          <t>P0122-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1509,27 +1509,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CIES-12636</t>
+          <t>CIES-16723</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 3</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0033</t>
+          <t>câmera do p0089 com galhos a frente</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>P0033-PCL-PK-CAR</t>
+          <t>P0089-PCL-PK-VIA</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1546,27 +1546,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CIES-12637</t>
+          <t>CIES-16724</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 3</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0290</t>
+          <t>câmera p0 139 embassada</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>P0290-PCL-PK-SER</t>
+          <t>P0039-PCL-PK-VVE</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1583,7 +1583,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CIES-12638</t>
+          <t>CIES-16725</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1593,7 +1593,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">CORRETIVA SITE P0076 </t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0150</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>P0076-PCL-PK-CAR</t>
+          <t>P0150-PCL-PK-FUN</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1620,7 +1620,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CIES-12639</t>
+          <t>CIES-16726</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1630,17 +1630,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0148 estão off-line </t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0157</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>P0148-PCL-PK-FUN</t>
+          <t>P0157-PCL-PK-FUN</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1650,14 +1650,14 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>FORA DO PRAZO</t>
+          <t>NO PRAZO</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CIES-12640</t>
+          <t>CIES-16727</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1667,17 +1667,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0147 estão off-line </t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0092</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>P0147-PCL-PK-FUN</t>
+          <t>P0092-PCL-PK-BAI</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1694,17 +1694,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CIES-12641</t>
+          <t>CIES-16728</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 3</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0095 estão off-line </t>
+          <t xml:space="preserve">câmera lpr 2 do p0 140 com fios a frente </t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1714,7 +1714,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>P0095-PCL-PK-AFO</t>
+          <t>P0140-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1731,27 +1731,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CIES-12644</t>
+          <t>CIES-16729</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 3</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0177</t>
+          <t xml:space="preserve">CÂMERA DO P0 118 CONT 2 COM OBSTRUÇÃO </t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>P0177-PK-VLS-SER</t>
+          <t>P0118-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1768,7 +1768,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CIES-12645</t>
+          <t>CIES-16738</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0141</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0039</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1788,7 +1788,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>P0141-PK-VLS-SER</t>
+          <t>P0039-PCL-PK-VVE</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1805,7 +1805,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CIES-12646</t>
+          <t>CIES-16739</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1815,7 +1815,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0133</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0034</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>P0133-PCL-PK-SER</t>
+          <t>P0034-PCL-PK-VVE</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1842,7 +1842,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>CIES-12648</t>
+          <t>CIES-16740</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1852,7 +1852,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0150</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0091</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>P0150-PCL-PK-FUN</t>
+          <t>P0091-PCL-PK-VIA</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1879,7 +1879,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CIES-12649</t>
+          <t>CIES-16741</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1889,7 +1889,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0129</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0124</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1899,7 +1899,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>P0129-PCL-PK-SER</t>
+          <t>P0124-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1916,7 +1916,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>CIES-12650</t>
+          <t>CIES-16742</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1926,7 +1926,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0290</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0122</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>P0290-PCL-PK-SER</t>
+          <t>P0122-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1953,32 +1953,32 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CIES-12652</t>
+          <t>CIES-16743</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 3</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0087</t>
+          <t xml:space="preserve"> CÂMERA DO P0 118 CONT 2 COM OBSTRUÇÃO </t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>P0087-PCL-PK-VIA</t>
+          <t>P0118-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>NO PRAZO</t>
+          <t>FORA DO PRAZO</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -1990,7 +1990,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CIES-12653</t>
+          <t>CIES-16744</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2000,17 +2000,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0090</t>
+          <t>camera cont 1 d p0001 virada</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>P0090-PCL-PK-VIA</t>
+          <t>P0001-PCL-PK-GRP</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2027,7 +2027,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>CIES-12654</t>
+          <t>CIES-16745</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2037,7 +2037,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>CORRETIVA SITE P0060</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0164</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2047,7 +2047,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>P0060-PCL-PK-CAR</t>
+          <t>P0164-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2064,7 +2064,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CIES-12672</t>
+          <t>CIES-16746</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2074,7 +2074,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0170</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0111</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -2084,7 +2084,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>P0170-PK-VLS-MIM</t>
+          <t>P0111-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2101,7 +2101,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>CIES-12673</t>
+          <t>CIES-16770</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2111,17 +2111,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0130</t>
+          <t xml:space="preserve">câmeras do p0036 fora de posicionamento </t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>P0130-PCL-PK-SER</t>
+          <t>P0036-PCL-PK-VVE</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2138,27 +2138,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>CIES-12702</t>
+          <t>CIES-16771</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Prioridade 1</t>
+          <t>Prioridade 3</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0198</t>
+          <t>câmera do p0045 sem identificação</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Service Desk Perkons</t>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>P0198-PK-VLS-GRP</t>
+          <t>P0045-PCL-PK-VVE</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2175,7 +2175,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>CIES-12712</t>
+          <t>CIES-16772</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2185,17 +2185,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0068 estão off-line   </t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0111</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>P0068-PCL-PK-CAR</t>
+          <t>P0111-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2212,7 +2212,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>CIES-12713</t>
+          <t>CIES-16789</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2222,17 +2222,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0068 estão off-line   </t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0035</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>P0069-PCL-PK-CAR</t>
+          <t>P0035-PCL-PK-CAR</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2249,7 +2249,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>CIES-12714</t>
+          <t>CIES-16790</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2259,17 +2259,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t xml:space="preserve">todas as câmeras do p0208 estão off-line   </t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0155</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+          <t>Service Desk Perkons</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>P0208-PK-VLS-SER</t>
+          <t>P0155-PCL-PK-FUN</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2286,7 +2286,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>CIES-12729</t>
+          <t>CIES-16791</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2323,7 +2323,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>CIES-12730</t>
+          <t>CIES-16792</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0120</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0091</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2343,7 +2343,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>P0120-PCL-PK-SER</t>
+          <t>P0091-PCL-PK-VIA</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2360,7 +2360,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>CIES-12731</t>
+          <t>CIES-16801</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0122</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0160</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2380,7 +2380,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>P0122-PCL-PK-SER</t>
+          <t>P0160-PCL-PK-FUN</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2397,7 +2397,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>CIES-12732</t>
+          <t>CIES-16802</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2407,7 +2407,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0129</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0118</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2417,7 +2417,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>P0129-PCL-PK-SER</t>
+          <t>P0118-PCL-PK-SER</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -2434,7 +2434,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>CIES-12733</t>
+          <t>CIES-16803</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2444,7 +2444,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0160</t>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0091</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>P0160-PCL-PK-FUN</t>
+          <t>P0091-PCL-PK-VIA</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2463,6 +2463,228 @@
         </is>
       </c>
       <c r="G55" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>CIES-16806</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0092</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>P0092-PCL-PK-BAI</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>CIES-16820</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Prioridade 3</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">câmera do p0 127 frontal toda branca </t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>P0127-PCL-PK-SER</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>CIES-16821</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Prioridade 3</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">câmera do p0 130 embaçada  </t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>CRISTIANA NEVES BATISTA MOREIRA</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>P0130-PCL-PK-SER</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>CIES-16854</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0152</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>P0152-PCL-PK-FUN</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>CIES-16855</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0157</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>P0157-PCL-PK-FUN</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>CIES-16856</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Prioridade 1</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>TODAS AS CÂMERAS DO SITE ESTÃO OFFLINE - P0091</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Service Desk Perkons</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>P0091-PCL-PK-VIA</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>NO PRAZO</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
         <is>
           <t>NO PRAZO</t>
         </is>

</xml_diff>